<commit_message>
Re-TL S00033, S00034, S00037
</commit_message>
<xml_diff>
--- a/tl/S00034.MES.BIN.xlsx
+++ b/tl/S00034.MES.BIN.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5227045F-047B-452D-BC14-04FCF9A63016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F596DA-C5EB-4D8E-8581-F75B050DEBC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="9810" windowWidth="45900" windowHeight="19845" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="18495" windowWidth="54585" windowHeight="12585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S00034.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="373">
   <si>
     <t>Status</t>
   </si>
@@ -86,7 +86,7 @@
     <t>11</t>
   </si>
   <si>
-    <t>...Kagerazaki Academy, third year......</t>
+    <t>…Hotarugasaki Academy, third year......</t>
   </si>
   <si>
     <t>13</t>
@@ -116,7 +116,7 @@
     <t>19</t>
   </si>
   <si>
-    <t>Well, it's my fault for not reading the documents closely...</t>
+    <t>...Well, it's my fault for not reading the documents closely…....</t>
   </si>
   <si>
     <t>21</t>
@@ -149,7 +149,7 @@
     <t>27</t>
   </si>
   <si>
-    <t>...student...</t>
+    <t>…Student…....</t>
   </si>
   <si>
     <t>...partner...</t>
@@ -158,7 +158,7 @@
     <t>29</t>
   </si>
   <si>
-    <t>Now that I think about it, I forgot to check what kind of person I'll be tutoring is...</t>
+    <t>Now that I think about it, I forgot to check what kind of person I'll be tutoring is….</t>
   </si>
   <si>
     <t>Now that I think about it, I forgot to check what kind of person the partner is...</t>
@@ -167,7 +167,7 @@
     <t>31</t>
   </si>
   <si>
-    <t>...ugh, what am I doing?</t>
+    <t>…What am I doing?</t>
   </si>
   <si>
     <t>...What am I doing?</t>
@@ -182,19 +182,19 @@
     <t>35</t>
   </si>
   <si>
-    <t>All that was written there was just the name "Mana Mizuki".</t>
+    <t>All that was written there was just the name &lt;c4"Mana Mizuki"&gt;.</t>
   </si>
   <si>
     <t>37</t>
   </si>
   <si>
-    <t>Mana Mizuki...</t>
+    <t>Mana Mizuki…....</t>
   </si>
   <si>
     <t>39</t>
   </si>
   <si>
-    <t>...She looks like a girl, but...</t>
+    <t>...She looks like a girl, but…....</t>
   </si>
   <si>
     <t>...She looks like a girl......</t>
@@ -203,13 +203,13 @@
     <t>41</t>
   </si>
   <si>
-    <t>Mizuki...</t>
+    <t>"Mizuki"</t>
   </si>
   <si>
     <t>43</t>
   </si>
   <si>
-    <t>...So this is the place......</t>
+    <t>...So this is the place…....</t>
   </si>
   <si>
     <t>45</t>
@@ -248,19 +248,19 @@
     <t>53</t>
   </si>
   <si>
-    <t>...I ring the doorbell but there's no response.</t>
+    <t>...I ring the doorbell, but there's no response.</t>
   </si>
   <si>
     <t>55</t>
   </si>
   <si>
-    <t>That's strange...</t>
+    <t>That's strange,</t>
   </si>
   <si>
     <t>57</t>
   </si>
   <si>
-    <t>There should be someone here...</t>
+    <t>there should be someone here…....</t>
   </si>
   <si>
     <t>59</t>
@@ -269,19 +269,22 @@
     <t>61</t>
   </si>
   <si>
-    <t>...Nobody's coming out......</t>
+    <t>...Nobody's coming out…....</t>
   </si>
   <si>
     <t>63</t>
   </si>
   <si>
+    <t>Maybe…they're not home…....</t>
+  </si>
+  <si>
     <t>Maybe they're not home......</t>
   </si>
   <si>
     <t>65</t>
   </si>
   <si>
-    <t>...What should I do...</t>
+    <t>...What should I do…....</t>
   </si>
   <si>
     <t>67</t>
@@ -578,12 +581,15 @@
     <t>145</t>
   </si>
   <si>
-    <t>"I said it's just me!</t>
+    <t>"I said, it's just me!</t>
   </si>
   <si>
     <t>147</t>
   </si>
   <si>
+    <t>She declares this as if it was a fact.</t>
+  </si>
+  <si>
     <t>She declared it as if it was a fact.</t>
   </si>
   <si>
@@ -698,7 +704,7 @@
     <t>181</t>
   </si>
   <si>
-    <t>And with full force too...</t>
+    <t>And with full force too…</t>
   </si>
   <si>
     <t>And with full force.</t>
@@ -719,6 +725,9 @@
     <t>187</t>
   </si>
   <si>
+    <t>…You…</t>
+  </si>
+  <si>
     <t>"...You...-"</t>
   </si>
   <si>
@@ -734,6 +743,9 @@
     <t>32</t>
   </si>
   <si>
+    <t>Mana</t>
+  </si>
+  <si>
     <t>"Mana."</t>
   </si>
   <si>
@@ -845,6 +857,9 @@
     <t>223</t>
   </si>
   <si>
+    <t>O-okay…...</t>
+  </si>
+  <si>
     <t>O...okay...</t>
   </si>
   <si>
@@ -974,9 +989,6 @@
     <t>259</t>
   </si>
   <si>
-    <t>"That's it for now. I'm getting tired. Good work. Bye now.</t>
-  </si>
-  <si>
     <t>"That's it for now. I'm getting tired. Good work. Goodbye.</t>
   </si>
   <si>
@@ -1001,7 +1013,7 @@
     <t>265</t>
   </si>
   <si>
-    <t>Hey, wait! What about the job interview I came here for?!</t>
+    <t>Hey, wait! What about the job interview I came here for!?</t>
   </si>
   <si>
     <t>"No, wait! I'm here for a job interview, but what about me!?</t>
@@ -1067,7 +1079,7 @@
     <t>283</t>
   </si>
   <si>
-    <t>Actually it's okay! My mom is just busy working! You can't talk with her because she's not home!</t>
+    <t>Never mind! My mom is just busy working! You can't talk with her because she's not home!</t>
   </si>
   <si>
     <t>...Yeah! Mom's busy with work today, so there's no way I can meet her!</t>
@@ -1115,7 +1127,13 @@
     <t>295</t>
   </si>
   <si>
+    <t>Go home quietly</t>
+  </si>
+  <si>
     <t>297</t>
+  </si>
+  <si>
+    <t>Persist</t>
   </si>
 </sst>
 </file>
@@ -1537,7 +1555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2588,10 +2608,10 @@
         <v>9</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>9</v>
@@ -2608,7 +2628,7 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>9</v>
@@ -2623,7 +2643,7 @@
         <v>9</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>9</v>
@@ -2640,7 +2660,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -2655,7 +2675,7 @@
         <v>9</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H35" s="5" t="s">
         <v>9</v>
@@ -2672,7 +2692,7 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>9</v>
@@ -2687,7 +2707,7 @@
         <v>9</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>9</v>
@@ -2704,7 +2724,7 @@
         <v>9</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -2719,7 +2739,7 @@
         <v>9</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H37" s="5" t="s">
         <v>9</v>
@@ -2736,7 +2756,7 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>9</v>
@@ -2748,10 +2768,10 @@
         <v>9</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>9</v>
@@ -2768,7 +2788,7 @@
         <v>9</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -2780,10 +2800,10 @@
         <v>9</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H39" s="5" t="s">
         <v>9</v>
@@ -2800,22 +2820,22 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>9</v>
@@ -2832,13 +2852,13 @@
         <v>9</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>9</v>
@@ -2847,7 +2867,7 @@
         <v>9</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H41" s="5" t="s">
         <v>9</v>
@@ -2864,7 +2884,7 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>9</v>
@@ -2879,7 +2899,7 @@
         <v>9</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H42" s="3" t="s">
         <v>9</v>
@@ -2896,13 +2916,13 @@
         <v>9</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>9</v>
@@ -2911,7 +2931,7 @@
         <v>9</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>9</v>
@@ -2928,7 +2948,7 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>9</v>
@@ -2943,7 +2963,7 @@
         <v>9</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>9</v>
@@ -2960,7 +2980,7 @@
         <v>9</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
@@ -2975,7 +2995,7 @@
         <v>9</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H45" s="5" t="s">
         <v>9</v>
@@ -2992,22 +3012,22 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E46" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>9</v>
@@ -3024,7 +3044,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -3039,7 +3059,7 @@
         <v>9</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>9</v>
@@ -3056,22 +3076,22 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>9</v>
@@ -3088,7 +3108,7 @@
         <v>9</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -3100,10 +3120,10 @@
         <v>9</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H49" s="5" t="s">
         <v>9</v>
@@ -3120,7 +3140,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>9</v>
@@ -3132,10 +3152,10 @@
         <v>9</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>9</v>
@@ -3152,22 +3172,22 @@
         <v>9</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H51" s="5" t="s">
         <v>9</v>
@@ -3184,7 +3204,7 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>9</v>
@@ -3199,7 +3219,7 @@
         <v>9</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>9</v>
@@ -3216,7 +3236,7 @@
         <v>9</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
@@ -3231,7 +3251,7 @@
         <v>9</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H53" s="5" t="s">
         <v>9</v>
@@ -3248,13 +3268,13 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>9</v>
@@ -3263,7 +3283,7 @@
         <v>9</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>9</v>
@@ -3280,7 +3300,7 @@
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -3295,7 +3315,7 @@
         <v>9</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H55" s="5" t="s">
         <v>9</v>
@@ -3312,22 +3332,22 @@
         <v>9</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E56" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>9</v>
@@ -3344,22 +3364,22 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H57" s="5" t="s">
         <v>9</v>
@@ -3376,13 +3396,13 @@
         <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>9</v>
@@ -3391,7 +3411,7 @@
         <v>9</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>9</v>
@@ -3408,22 +3428,22 @@
         <v>9</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H59" s="5" t="s">
         <v>9</v>
@@ -3440,7 +3460,7 @@
         <v>9</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>9</v>
@@ -3452,10 +3472,10 @@
         <v>9</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>9</v>
@@ -3472,22 +3492,22 @@
         <v>9</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H61" s="5" t="s">
         <v>9</v>
@@ -3504,13 +3524,13 @@
         <v>9</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E62" s="2" t="s">
         <v>9</v>
@@ -3519,7 +3539,7 @@
         <v>9</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>9</v>
@@ -3536,13 +3556,13 @@
         <v>9</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>9</v>
@@ -3551,7 +3571,7 @@
         <v>9</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>9</v>
@@ -3568,22 +3588,22 @@
         <v>9</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>9</v>
@@ -3600,13 +3620,13 @@
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E65" s="4" t="s">
         <v>9</v>
@@ -3615,7 +3635,7 @@
         <v>9</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H65" s="5" t="s">
         <v>9</v>
@@ -3632,7 +3652,7 @@
         <v>9</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>9</v>
@@ -3647,7 +3667,7 @@
         <v>9</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>9</v>
@@ -3664,7 +3684,7 @@
         <v>9</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
@@ -3679,7 +3699,7 @@
         <v>9</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H67" s="5" t="s">
         <v>9</v>
@@ -3696,7 +3716,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>9</v>
@@ -3708,10 +3728,10 @@
         <v>9</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>9</v>
@@ -3728,7 +3748,7 @@
         <v>9</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>9</v>
@@ -3743,7 +3763,7 @@
         <v>9</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H69" s="5" t="s">
         <v>9</v>
@@ -3760,7 +3780,7 @@
         <v>9</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>9</v>
@@ -3772,10 +3792,10 @@
         <v>9</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>9</v>
@@ -3792,13 +3812,13 @@
         <v>9</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E71" s="4" t="s">
         <v>9</v>
@@ -3807,7 +3827,7 @@
         <v>9</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>9</v>
@@ -3824,13 +3844,13 @@
         <v>9</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E72" s="2" t="s">
         <v>9</v>
@@ -3839,7 +3859,7 @@
         <v>9</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>9</v>
@@ -3856,13 +3876,13 @@
         <v>9</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E73" s="4" t="s">
         <v>9</v>
@@ -3871,7 +3891,7 @@
         <v>9</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H73" s="5" t="s">
         <v>9</v>
@@ -3888,13 +3908,13 @@
         <v>9</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E74" s="2" t="s">
         <v>9</v>
@@ -3903,7 +3923,7 @@
         <v>9</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H74" s="3" t="s">
         <v>9</v>
@@ -3920,7 +3940,7 @@
         <v>9</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>9</v>
@@ -3932,10 +3952,10 @@
         <v>9</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>9</v>
+        <v>190</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H75" s="5" t="s">
         <v>9</v>
@@ -3952,13 +3972,13 @@
         <v>9</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>9</v>
@@ -3967,7 +3987,7 @@
         <v>9</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>9</v>
@@ -3984,7 +4004,7 @@
         <v>9</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>9</v>
@@ -3999,7 +4019,7 @@
         <v>9</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="H77" s="5" t="s">
         <v>9</v>
@@ -4016,7 +4036,7 @@
         <v>9</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>9</v>
@@ -4031,7 +4051,7 @@
         <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>9</v>
@@ -4048,7 +4068,7 @@
         <v>9</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>9</v>
@@ -4063,7 +4083,7 @@
         <v>9</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H79" s="5" t="s">
         <v>9</v>
@@ -4080,7 +4100,7 @@
         <v>9</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>9</v>
@@ -4095,7 +4115,7 @@
         <v>9</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>9</v>
@@ -4112,13 +4132,13 @@
         <v>9</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E81" s="4" t="s">
         <v>9</v>
@@ -4127,7 +4147,7 @@
         <v>9</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H81" s="5" t="s">
         <v>9</v>
@@ -4144,7 +4164,7 @@
         <v>9</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>9</v>
@@ -4159,7 +4179,7 @@
         <v>9</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H82" s="3" t="s">
         <v>9</v>
@@ -4176,22 +4196,22 @@
         <v>9</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E83" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F83" s="4" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H83" s="5" t="s">
         <v>9</v>
@@ -4208,13 +4228,13 @@
         <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>9</v>
@@ -4223,7 +4243,7 @@
         <v>9</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>9</v>
@@ -4240,7 +4260,7 @@
         <v>9</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>9</v>
@@ -4252,10 +4272,10 @@
         <v>9</v>
       </c>
       <c r="F85" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="H85" s="5" t="s">
         <v>9</v>
@@ -4272,22 +4292,22 @@
         <v>9</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>9</v>
@@ -4304,7 +4324,7 @@
         <v>9</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>9</v>
@@ -4319,7 +4339,7 @@
         <v>9</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="H87" s="5" t="s">
         <v>9</v>
@@ -4336,7 +4356,7 @@
         <v>9</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>9</v>
@@ -4351,7 +4371,7 @@
         <v>9</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>9</v>
@@ -4368,7 +4388,7 @@
         <v>9</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>9</v>
@@ -4383,7 +4403,7 @@
         <v>9</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="H89" s="5" t="s">
         <v>9</v>
@@ -4400,7 +4420,7 @@
         <v>9</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>9</v>
@@ -4415,7 +4435,7 @@
         <v>9</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>9</v>
@@ -4432,7 +4452,7 @@
         <v>9</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>9</v>
@@ -4444,10 +4464,10 @@
         <v>9</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>9</v>
@@ -4464,7 +4484,7 @@
         <v>9</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>9</v>
@@ -4476,10 +4496,10 @@
         <v>9</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>9</v>
@@ -4496,7 +4516,7 @@
         <v>9</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>9</v>
@@ -4511,7 +4531,7 @@
         <v>9</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H93" s="5" t="s">
         <v>9</v>
@@ -4528,7 +4548,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C94" s="2" t="s">
         <v>9</v>
@@ -4543,7 +4563,7 @@
         <v>9</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>9</v>
@@ -4560,22 +4580,22 @@
         <v>9</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E95" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F95" s="4" t="s">
-        <v>9</v>
+        <v>236</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>9</v>
@@ -4592,7 +4612,7 @@
         <v>9</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C96" s="2" t="s">
         <v>9</v>
@@ -4607,7 +4627,7 @@
         <v>9</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H96" s="3" t="s">
         <v>9</v>
@@ -4624,13 +4644,13 @@
         <v>9</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>9</v>
@@ -4639,7 +4659,7 @@
         <v>9</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="H97" s="5" t="s">
         <v>9</v>
@@ -4656,7 +4676,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C98" s="2" t="s">
         <v>9</v>
@@ -4671,7 +4691,7 @@
         <v>9</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="H98" s="3" t="s">
         <v>9</v>
@@ -4688,22 +4708,22 @@
         <v>9</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E99" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F99" s="4" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="H99" s="5" t="s">
         <v>9</v>
@@ -4720,7 +4740,7 @@
         <v>9</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="C100" s="2" t="s">
         <v>9</v>
@@ -4735,7 +4755,7 @@
         <v>9</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>9</v>
@@ -4752,7 +4772,7 @@
         <v>9</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>9</v>
@@ -4767,7 +4787,7 @@
         <v>9</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="H101" s="5" t="s">
         <v>9</v>
@@ -4784,13 +4804,13 @@
         <v>9</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C102" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>9</v>
@@ -4799,7 +4819,7 @@
         <v>9</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>9</v>
@@ -4816,22 +4836,22 @@
         <v>9</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E103" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F103" s="4" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="H103" s="5" t="s">
         <v>9</v>
@@ -4848,7 +4868,7 @@
         <v>9</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C104" s="2" t="s">
         <v>9</v>
@@ -4860,10 +4880,10 @@
         <v>9</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>9</v>
@@ -4880,13 +4900,13 @@
         <v>9</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E105" s="4" t="s">
         <v>9</v>
@@ -4895,7 +4915,7 @@
         <v>9</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="H105" s="5" t="s">
         <v>9</v>
@@ -4912,7 +4932,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>9</v>
@@ -4927,7 +4947,7 @@
         <v>9</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>9</v>
@@ -4944,7 +4964,7 @@
         <v>9</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>9</v>
@@ -4959,7 +4979,7 @@
         <v>9</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="H107" s="5" t="s">
         <v>9</v>
@@ -4976,7 +4996,7 @@
         <v>9</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>9</v>
@@ -4991,7 +5011,7 @@
         <v>9</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>9</v>
@@ -5008,13 +5028,13 @@
         <v>9</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D109" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E109" s="4" t="s">
         <v>9</v>
@@ -5023,7 +5043,7 @@
         <v>9</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H109" s="5" t="s">
         <v>9</v>
@@ -5040,7 +5060,7 @@
         <v>9</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>9</v>
@@ -5052,10 +5072,10 @@
         <v>9</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>9</v>
@@ -5072,7 +5092,7 @@
         <v>9</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>9</v>
@@ -5084,10 +5104,10 @@
         <v>9</v>
       </c>
       <c r="F111" s="4" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="H111" s="5" t="s">
         <v>9</v>
@@ -5104,13 +5124,13 @@
         <v>9</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>9</v>
@@ -5119,7 +5139,7 @@
         <v>9</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>9</v>
@@ -5136,22 +5156,22 @@
         <v>9</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D113" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E113" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F113" s="4" t="s">
-        <v>9</v>
+        <v>280</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="H113" s="5" t="s">
         <v>9</v>
@@ -5168,7 +5188,7 @@
         <v>9</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>9</v>
@@ -5180,10 +5200,10 @@
         <v>9</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="H114" s="3" t="s">
         <v>9</v>
@@ -5200,7 +5220,7 @@
         <v>9</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>9</v>
@@ -5212,10 +5232,10 @@
         <v>9</v>
       </c>
       <c r="F115" s="4" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="H115" s="5" t="s">
         <v>9</v>
@@ -5232,22 +5252,22 @@
         <v>9</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="H116" s="3" t="s">
         <v>9</v>
@@ -5264,13 +5284,13 @@
         <v>9</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>9</v>
@@ -5279,7 +5299,7 @@
         <v>9</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="H117" s="5" t="s">
         <v>9</v>
@@ -5296,7 +5316,7 @@
         <v>9</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>9</v>
@@ -5311,7 +5331,7 @@
         <v>9</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
       <c r="H118" s="3" t="s">
         <v>9</v>
@@ -5328,7 +5348,7 @@
         <v>9</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>9</v>
@@ -5343,7 +5363,7 @@
         <v>9</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>291</v>
+        <v>296</v>
       </c>
       <c r="H119" s="5" t="s">
         <v>9</v>
@@ -5360,22 +5380,22 @@
         <v>9</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>292</v>
+        <v>297</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>293</v>
+        <v>298</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>294</v>
+        <v>299</v>
       </c>
       <c r="H120" s="3" t="s">
         <v>9</v>
@@ -5392,13 +5412,13 @@
         <v>9</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E121" s="4" t="s">
         <v>9</v>
@@ -5407,7 +5427,7 @@
         <v>9</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>296</v>
+        <v>301</v>
       </c>
       <c r="H121" s="5" t="s">
         <v>9</v>
@@ -5424,22 +5444,22 @@
         <v>9</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>297</v>
+        <v>302</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>298</v>
+        <v>303</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="H122" s="3" t="s">
         <v>9</v>
@@ -5456,22 +5476,22 @@
         <v>9</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E123" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>301</v>
+        <v>306</v>
       </c>
       <c r="G123" s="5" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="H123" s="5" t="s">
         <v>9</v>
@@ -5488,13 +5508,13 @@
         <v>9</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>9</v>
@@ -5503,7 +5523,7 @@
         <v>9</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="H124" s="3" t="s">
         <v>9</v>
@@ -5520,22 +5540,22 @@
         <v>9</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E125" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
       <c r="G125" s="5" t="s">
-        <v>307</v>
+        <v>312</v>
       </c>
       <c r="H125" s="5" t="s">
         <v>9</v>
@@ -5552,22 +5572,22 @@
         <v>9</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>308</v>
+        <v>313</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>309</v>
+        <v>314</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>9</v>
@@ -5584,13 +5604,13 @@
         <v>9</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E127" s="4" t="s">
         <v>9</v>
@@ -5599,7 +5619,7 @@
         <v>9</v>
       </c>
       <c r="G127" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H127" s="5" t="s">
         <v>9</v>
@@ -5616,7 +5636,7 @@
         <v>9</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>9</v>
@@ -5631,7 +5651,7 @@
         <v>9</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="H128" s="3" t="s">
         <v>9</v>
@@ -5648,13 +5668,13 @@
         <v>9</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E129" s="4" t="s">
         <v>9</v>
@@ -5663,7 +5683,7 @@
         <v>9</v>
       </c>
       <c r="G129" s="5" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="H129" s="5" t="s">
         <v>9</v>
@@ -5680,13 +5700,13 @@
         <v>9</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>9</v>
@@ -5695,7 +5715,7 @@
         <v>9</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="H130" s="3" t="s">
         <v>9</v>
@@ -5712,22 +5732,22 @@
         <v>9</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E131" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="G131" s="5" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="H131" s="5" t="s">
         <v>9</v>
@@ -5744,22 +5764,22 @@
         <v>9</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>9</v>
@@ -5776,7 +5796,7 @@
         <v>9</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>9</v>
@@ -5788,10 +5808,10 @@
         <v>9</v>
       </c>
       <c r="F133" s="4" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G133" s="5" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="H133" s="5" t="s">
         <v>9</v>
@@ -5808,22 +5828,22 @@
         <v>9</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E134" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>9</v>
@@ -5840,7 +5860,7 @@
         <v>9</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>9</v>
@@ -5855,7 +5875,7 @@
         <v>9</v>
       </c>
       <c r="G135" s="5" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="H135" s="5" t="s">
         <v>9</v>
@@ -5872,22 +5892,22 @@
         <v>9</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E136" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="H136" s="3" t="s">
         <v>9</v>
@@ -5904,13 +5924,13 @@
         <v>9</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E137" s="4" t="s">
         <v>9</v>
@@ -5919,7 +5939,7 @@
         <v>9</v>
       </c>
       <c r="G137" s="5" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="H137" s="5" t="s">
         <v>9</v>
@@ -5936,13 +5956,13 @@
         <v>9</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>9</v>
@@ -5951,7 +5971,7 @@
         <v>9</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="H138" s="3" t="s">
         <v>9</v>
@@ -5968,13 +5988,13 @@
         <v>9</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C139" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D139" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E139" s="4" t="s">
         <v>9</v>
@@ -5983,7 +6003,7 @@
         <v>9</v>
       </c>
       <c r="G139" s="5" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="H139" s="5" t="s">
         <v>9</v>
@@ -6000,7 +6020,7 @@
         <v>9</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C140" s="2" t="s">
         <v>9</v>
@@ -6015,7 +6035,7 @@
         <v>9</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="H140" s="3" t="s">
         <v>9</v>
@@ -6032,22 +6052,22 @@
         <v>9</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E141" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F141" s="4" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="G141" s="5" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="H141" s="5" t="s">
         <v>9</v>
@@ -6064,22 +6084,22 @@
         <v>9</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>9</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="H142" s="3" t="s">
         <v>9</v>
@@ -6096,22 +6116,22 @@
         <v>9</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E143" s="4" t="s">
         <v>9</v>
       </c>
       <c r="F143" s="4" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="G143" s="5" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="H143" s="5" t="s">
         <v>9</v>
@@ -6128,7 +6148,7 @@
         <v>9</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>9</v>
@@ -6140,10 +6160,10 @@
         <v>9</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="H144" s="3" t="s">
         <v>9</v>
@@ -6160,7 +6180,7 @@
         <v>9</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="C145" s="4" t="s">
         <v>9</v>
@@ -6175,7 +6195,7 @@
         <v>9</v>
       </c>
       <c r="G145" s="5" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="H145" s="5" t="s">
         <v>9</v>
@@ -6192,13 +6212,13 @@
         <v>9</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>103</v>
+        <v>242</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>9</v>
@@ -6207,7 +6227,7 @@
         <v>9</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="H146" s="3" t="s">
         <v>9</v>
@@ -6224,7 +6244,7 @@
         <v>9</v>
       </c>
       <c r="B147" s="4" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="C147" s="4" t="s">
         <v>9</v>
@@ -6236,10 +6256,10 @@
         <v>9</v>
       </c>
       <c r="F147" s="4" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="G147" s="5" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="H147" s="5" t="s">
         <v>9</v>
@@ -6256,7 +6276,7 @@
         <v>9</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>9</v>
@@ -6268,10 +6288,10 @@
         <v>9</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="H148" s="3" t="s">
         <v>9</v>
@@ -6288,7 +6308,7 @@
         <v>9</v>
       </c>
       <c r="B149" s="4" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>9</v>
@@ -6303,7 +6323,7 @@
         <v>9</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>9</v>
+        <v>370</v>
       </c>
       <c r="H149" s="5" t="s">
         <v>9</v>
@@ -6320,7 +6340,7 @@
         <v>9</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="C150" s="2" t="s">
         <v>9</v>
@@ -6335,7 +6355,7 @@
         <v>9</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>9</v>
+        <v>372</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>9</v>

</xml_diff>